<commit_message>
Actualizacion del componente de seguimiento.HRR
</commit_message>
<xml_diff>
--- a/database/seeders/Usuarios.xlsx
+++ b/database/seeders/Usuarios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\XAMPPROD\htdocs\GITComponentes\Seguimiento\database\seeders\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harold\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105ED7C0-EDA6-45C9-8E48-02481F79B1DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A9A10F-3F8E-419E-94D5-14C61C7A6378}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{927018C0-BB9F-433A-9F90-4096039434DC}"/>
   </bookViews>
@@ -20,19 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="150">
   <si>
     <t>nombre</t>
   </si>
@@ -466,10 +459,22 @@
     <t>plataforma_id</t>
   </si>
   <si>
-    <t>José Antonio Mercado Sanchez</t>
-  </si>
-  <si>
-    <t>mercadozamora@hotmail.com</t>
+    <t>Berenice Antonio Cándido</t>
+  </si>
+  <si>
+    <t>acb830927@gmail.com</t>
+  </si>
+  <si>
+    <t>José Luis Hernández Maldonado</t>
+  </si>
+  <si>
+    <t>pepeluismaldonado8@gmail.com</t>
+  </si>
+  <si>
+    <t>Maricela López Ventura</t>
+  </si>
+  <si>
+    <t>maricela.love.07@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -608,7 +613,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -695,6 +700,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1020,10 +1034,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{850591BD-AB77-48DF-A9A3-0C3060FEC0A7}">
-  <dimension ref="A1:G66"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="H69" sqref="H69"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1543,80 +1557,78 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="C23" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="D23" s="27">
-        <v>122130</v>
-      </c>
-      <c r="E23" s="27" t="s">
-        <v>138</v>
-      </c>
-      <c r="F23" s="27" t="s">
-        <v>139</v>
-      </c>
-      <c r="G23" s="27">
-        <v>1590</v>
-      </c>
+      <c r="A23" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B23" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D23" s="26">
+        <v>122120</v>
+      </c>
+      <c r="E23" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="F23" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="G23" s="26"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D24" s="27">
         <v>122130</v>
       </c>
       <c r="E24" s="27" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F24" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G24" s="27">
-        <v>1591</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="C25" s="22" t="s">
-        <v>135</v>
+        <v>92</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>134</v>
       </c>
       <c r="D25" s="27">
         <v>122130</v>
       </c>
       <c r="E25" s="27" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F25" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G25" s="27">
-        <v>1592</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C26" s="22" t="s">
         <v>135</v>
@@ -1631,15 +1643,15 @@
         <v>141</v>
       </c>
       <c r="G26" s="27">
-        <v>1593</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C27" s="22" t="s">
         <v>135</v>
@@ -1654,15 +1666,15 @@
         <v>141</v>
       </c>
       <c r="G27" s="27">
-        <v>1594</v>
+        <v>1593</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C28" s="22" t="s">
         <v>135</v>
@@ -1677,61 +1689,61 @@
         <v>141</v>
       </c>
       <c r="G28" s="27">
-        <v>1595</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="C29" s="21" t="s">
-        <v>134</v>
+        <v>96</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>135</v>
       </c>
       <c r="D29" s="27">
         <v>122130</v>
       </c>
       <c r="E29" s="27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F29" s="27" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G29" s="27">
-        <v>1596</v>
+        <v>1595</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="C30" s="22" t="s">
-        <v>135</v>
+        <v>97</v>
+      </c>
+      <c r="C30" s="21" t="s">
+        <v>134</v>
       </c>
       <c r="D30" s="27">
         <v>122130</v>
       </c>
       <c r="E30" s="27" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F30" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G30" s="27">
-        <v>1597</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C31" s="22" t="s">
         <v>135</v>
@@ -1746,15 +1758,15 @@
         <v>141</v>
       </c>
       <c r="G31" s="27">
-        <v>1598</v>
+        <v>1597</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C32" s="22" t="s">
         <v>135</v>
@@ -1769,15 +1781,15 @@
         <v>141</v>
       </c>
       <c r="G32" s="27">
-        <v>1599</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C33" s="22" t="s">
         <v>135</v>
@@ -1792,107 +1804,105 @@
         <v>141</v>
       </c>
       <c r="G33" s="27">
+        <v>1599</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="D34" s="27">
+        <v>122130</v>
+      </c>
+      <c r="E34" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="F34" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="G34" s="27">
         <v>1600</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="B34" s="32" t="s">
-        <v>102</v>
-      </c>
-      <c r="C34" s="33" t="s">
-        <v>133</v>
-      </c>
-      <c r="D34" s="30">
-        <v>122210</v>
-      </c>
-      <c r="E34" s="30" t="s">
-        <v>138</v>
-      </c>
-      <c r="F34" s="30" t="s">
-        <v>139</v>
-      </c>
-      <c r="G34" s="30">
-        <v>1601</v>
-      </c>
-    </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="B35" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="C35" s="33" t="s">
-        <v>134</v>
-      </c>
-      <c r="D35" s="30">
-        <v>122210</v>
-      </c>
-      <c r="E35" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="F35" s="30" t="s">
-        <v>140</v>
-      </c>
-      <c r="G35" s="30">
-        <v>1602</v>
-      </c>
+      <c r="A35" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B35" s="35" t="s">
+        <v>147</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="D35" s="27">
+        <v>122130</v>
+      </c>
+      <c r="E35" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="F35" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="G35" s="27"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B36" s="32" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C36" s="33" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D36" s="30">
         <v>122210</v>
       </c>
       <c r="E36" s="30" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F36" s="30" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G36" s="30">
-        <v>1603</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B37" s="32" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C37" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D37" s="30">
         <v>122210</v>
       </c>
       <c r="E37" s="30" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F37" s="30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G37" s="30">
-        <v>1604</v>
+        <v>1602</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B38" s="32" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C38" s="33" t="s">
         <v>135</v>
@@ -1907,15 +1917,15 @@
         <v>141</v>
       </c>
       <c r="G38" s="30">
-        <v>1605</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="31" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B39" s="32" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C39" s="33" t="s">
         <v>135</v>
@@ -1930,38 +1940,38 @@
         <v>141</v>
       </c>
       <c r="G39" s="30">
-        <v>1606</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="31" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B40" s="32" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C40" s="33" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D40" s="30">
         <v>122210</v>
       </c>
       <c r="E40" s="30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F40" s="30" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G40" s="30">
-        <v>1607</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="31" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B41" s="32" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C41" s="33" t="s">
         <v>135</v>
@@ -1976,38 +1986,38 @@
         <v>141</v>
       </c>
       <c r="G41" s="30">
-        <v>1608</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="31" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B42" s="32" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C42" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D42" s="30">
         <v>122210</v>
       </c>
       <c r="E42" s="30" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F42" s="30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G42" s="30">
-        <v>1609</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B43" s="32" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C43" s="33" t="s">
         <v>135</v>
@@ -2022,15 +2032,15 @@
         <v>141</v>
       </c>
       <c r="G43" s="30">
-        <v>1610</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="31" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B44" s="32" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C44" s="33" t="s">
         <v>135</v>
@@ -2045,130 +2055,130 @@
         <v>141</v>
       </c>
       <c r="G44" s="30">
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="C45" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="D45" s="30">
+        <v>122210</v>
+      </c>
+      <c r="E45" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="F45" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="G45" s="30">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B46" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="C46" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="D46" s="30">
+        <v>122210</v>
+      </c>
+      <c r="E46" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="F46" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="G46" s="30">
         <v>1611</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B45" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="C45" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="D45" s="28">
-        <v>122220</v>
-      </c>
-      <c r="E45" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="F45" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="G45" s="28">
-        <v>1612</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B46" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="C46" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="D46" s="28">
-        <v>122220</v>
-      </c>
-      <c r="E46" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="F46" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="G46" s="28">
-        <v>1613</v>
-      </c>
-    </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B47" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="C47" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="D47" s="28">
-        <v>122220</v>
-      </c>
-      <c r="E47" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="F47" s="28" t="s">
-        <v>141</v>
-      </c>
-      <c r="G47" s="28">
-        <v>1614</v>
+      <c r="A47" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="B47" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="C47" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="D47" s="30">
+        <v>122210</v>
+      </c>
+      <c r="E47" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="F47" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="G47" s="30">
+        <v>1611</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C48" s="23" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D48" s="28">
         <v>122220</v>
       </c>
       <c r="E48" s="28" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F48" s="28" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G48" s="28">
-        <v>1615</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C49" s="23" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D49" s="28">
         <v>122220</v>
       </c>
       <c r="E49" s="28" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F49" s="28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G49" s="28">
-        <v>1616</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C50" s="23" t="s">
         <v>135</v>
@@ -2183,38 +2193,38 @@
         <v>141</v>
       </c>
       <c r="G50" s="28">
-        <v>1617</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C51" s="23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D51" s="28">
         <v>122220</v>
       </c>
       <c r="E51" s="28" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F51" s="28" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G51" s="28">
-        <v>1618</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B52" s="14" t="s">
-        <v>142</v>
+        <v>53</v>
+      </c>
+      <c r="B52" s="13" t="s">
+        <v>117</v>
       </c>
       <c r="C52" s="23" t="s">
         <v>135</v>
@@ -2229,15 +2239,15 @@
         <v>141</v>
       </c>
       <c r="G52" s="28">
-        <v>1619</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C53" s="23" t="s">
         <v>135</v>
@@ -2252,38 +2262,38 @@
         <v>141</v>
       </c>
       <c r="G53" s="28">
-        <v>1620</v>
+        <v>1617</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C54" s="23" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D54" s="28">
         <v>122220</v>
       </c>
       <c r="E54" s="28" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F54" s="28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G54" s="28">
-        <v>1621</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B55" s="13" t="s">
-        <v>122</v>
+        <v>56</v>
+      </c>
+      <c r="B55" s="14" t="s">
+        <v>142</v>
       </c>
       <c r="C55" s="23" t="s">
         <v>135</v>
@@ -2298,153 +2308,153 @@
         <v>141</v>
       </c>
       <c r="G55" s="28">
+        <v>1619</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="C56" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="D56" s="28">
+        <v>122220</v>
+      </c>
+      <c r="E56" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="F56" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="G56" s="28">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B57" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C57" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="D57" s="28">
+        <v>122220</v>
+      </c>
+      <c r="E57" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="F57" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="G57" s="28">
+        <v>1621</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B58" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="C58" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="D58" s="28">
+        <v>122220</v>
+      </c>
+      <c r="E58" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="F58" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="G58" s="28">
         <v>1622</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B56" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="C56" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="D56" s="29">
-        <v>122230</v>
-      </c>
-      <c r="E56" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="F56" s="29" t="s">
-        <v>139</v>
-      </c>
-      <c r="G56" s="29">
-        <v>1623</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B57" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="C57" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="D57" s="29">
-        <v>122230</v>
-      </c>
-      <c r="E57" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="F57" s="29" t="s">
-        <v>140</v>
-      </c>
-      <c r="G57" s="29">
-        <v>1624</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B58" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="C58" s="24" t="s">
-        <v>137</v>
-      </c>
-      <c r="D58" s="29">
-        <v>122230</v>
-      </c>
-      <c r="E58" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="F58" s="29" t="s">
-        <v>141</v>
-      </c>
-      <c r="G58" s="29">
-        <v>1625</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C59" s="24" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D59" s="29">
         <v>122230</v>
       </c>
       <c r="E59" s="29" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F59" s="29" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G59" s="29">
-        <v>1626</v>
+        <v>1623</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C60" s="24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D60" s="29">
         <v>122230</v>
       </c>
       <c r="E60" s="29" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F60" s="29" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G60" s="29">
-        <v>1627</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C61" s="24" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D61" s="29">
         <v>122230</v>
       </c>
       <c r="E61" s="29" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F61" s="29" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G61" s="29">
-        <v>1628</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C62" s="24" t="s">
         <v>137</v>
@@ -2459,15 +2469,15 @@
         <v>141</v>
       </c>
       <c r="G62" s="29">
-        <v>1629</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C63" s="24" t="s">
         <v>137</v>
@@ -2482,38 +2492,38 @@
         <v>141</v>
       </c>
       <c r="G63" s="29">
-        <v>1630</v>
+        <v>1627</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C64" s="24" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D64" s="29">
         <v>122230</v>
       </c>
       <c r="E64" s="29" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F64" s="29" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G64" s="29">
-        <v>1631</v>
+        <v>1628</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C65" s="24" t="s">
         <v>137</v>
@@ -2528,15 +2538,15 @@
         <v>141</v>
       </c>
       <c r="G65" s="29">
-        <v>1632</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>144</v>
+        <v>67</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="C66" s="24" t="s">
         <v>137</v>
@@ -2551,7 +2561,53 @@
         <v>141</v>
       </c>
       <c r="G66" s="29">
-        <v>1651</v>
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B67" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="C67" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="D67" s="29">
+        <v>122230</v>
+      </c>
+      <c r="E67" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="F67" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="G67" s="29">
+        <v>1631</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B68" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C68" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="D68" s="29">
+        <v>122230</v>
+      </c>
+      <c r="E68" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="F68" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="G68" s="29">
+        <v>1632</v>
       </c>
     </row>
   </sheetData>
@@ -2573,50 +2629,52 @@
     <hyperlink ref="B18" r:id="rId15" xr:uid="{C980D029-3C80-42AF-8765-7B1B8975F8E8}"/>
     <hyperlink ref="B14" r:id="rId16" xr:uid="{76E74780-6902-456A-B091-8C3EFDCFF4F2}"/>
     <hyperlink ref="B19" r:id="rId17" xr:uid="{95DDDBEC-42FE-47D0-8609-4E5A207D6E83}"/>
-    <hyperlink ref="B23" r:id="rId18" xr:uid="{926C4943-E630-4939-84A2-BEFC74A5F225}"/>
-    <hyperlink ref="B33" r:id="rId19" xr:uid="{7A5C2798-8BE5-4E96-BDEF-28F7CD2E738F}"/>
-    <hyperlink ref="B28" r:id="rId20" xr:uid="{4C7EFCDB-0E77-4C97-ACE6-C0CE8C394D37}"/>
-    <hyperlink ref="B31" r:id="rId21" xr:uid="{26F4AAB3-FFF1-4E0E-BF78-C8093E37AFBD}"/>
-    <hyperlink ref="B26" r:id="rId22" xr:uid="{13911792-9821-4E95-97DC-85E9B887C511}"/>
-    <hyperlink ref="B27" r:id="rId23" xr:uid="{69E5226C-7630-4695-9C81-A26D1377DE88}"/>
-    <hyperlink ref="B30" r:id="rId24" xr:uid="{CECD053F-7FD3-4B64-A49A-5D9C5A5F3BF9}"/>
-    <hyperlink ref="B29" r:id="rId25" xr:uid="{07B1DA00-5CF5-4122-9A5B-999FDE6C29EB}"/>
-    <hyperlink ref="B24" r:id="rId26" xr:uid="{5D22632C-FEEF-46B7-9865-41DA5B5CFDB3}"/>
-    <hyperlink ref="B32" r:id="rId27" xr:uid="{94D658C0-A0FE-4BF5-A204-C13F43B26FA9}"/>
-    <hyperlink ref="B25" r:id="rId28" xr:uid="{7C76A1DF-0C89-476C-8887-065E272C5483}"/>
-    <hyperlink ref="B34" r:id="rId29" xr:uid="{91F877AB-DA05-47DE-AA82-82BDE2FECF1D}"/>
-    <hyperlink ref="B43" r:id="rId30" xr:uid="{E80CAB3F-FB06-4D2A-BDC5-C95FF9ED0484}"/>
-    <hyperlink ref="B40" r:id="rId31" xr:uid="{F26B1534-C4A9-4963-967B-4D5E96E36851}"/>
-    <hyperlink ref="B44" r:id="rId32" xr:uid="{A82F6207-BA99-4836-8841-34BAE60666F0}"/>
-    <hyperlink ref="B36" r:id="rId33" xr:uid="{D84DD9F0-2D54-4A2C-879F-8C72F1F45A6E}"/>
-    <hyperlink ref="B37" r:id="rId34" xr:uid="{74083F87-F085-4AB8-8EA4-CD2E4611AD88}"/>
-    <hyperlink ref="B35" r:id="rId35" xr:uid="{5669B6F1-A30D-4310-8B87-82A6CDCC48B6}"/>
-    <hyperlink ref="B38" r:id="rId36" xr:uid="{96086732-E496-4DBB-8FA1-E150E110C6B7}"/>
-    <hyperlink ref="B41" r:id="rId37" xr:uid="{81AA84CD-D665-447C-823E-48B3E248604A}"/>
-    <hyperlink ref="B39" r:id="rId38" xr:uid="{C8935CA7-3220-467F-B000-6149E5E058D8}"/>
-    <hyperlink ref="B42" r:id="rId39" xr:uid="{474CDAE7-FC2C-4D4A-B7A1-C15D3453707C}"/>
-    <hyperlink ref="B45" r:id="rId40" xr:uid="{9576E6D8-C736-4763-91C8-7E183557C4C5}"/>
-    <hyperlink ref="B46" r:id="rId41" xr:uid="{A195B2E4-268B-4E5A-8FB4-56B97F8E4B99}"/>
-    <hyperlink ref="B47" r:id="rId42" xr:uid="{4BC7E6B9-1EE9-4FD4-BC5F-59BA867871B3}"/>
-    <hyperlink ref="B48" r:id="rId43" xr:uid="{589630DE-5DAD-45EC-8F36-D47477C02C73}"/>
-    <hyperlink ref="B49" r:id="rId44" xr:uid="{1DEFFFFE-C0A9-4491-A8DF-1834C0DEC3C1}"/>
-    <hyperlink ref="B50" r:id="rId45" xr:uid="{3EFBB842-4AFA-4A49-A1DF-C64565E21D5E}"/>
-    <hyperlink ref="B51" r:id="rId46" xr:uid="{AE4CC454-C550-4A47-96DE-5B64F3548C49}"/>
-    <hyperlink ref="B52" r:id="rId47" xr:uid="{DB8B1B41-3C6E-4F7F-9919-E2A0B1161647}"/>
-    <hyperlink ref="B53" r:id="rId48" xr:uid="{E6BEDB91-7182-4204-A234-9C695262B83B}"/>
-    <hyperlink ref="B54" r:id="rId49" xr:uid="{9F11431B-223D-4F6D-B269-253E92D3D8E2}"/>
-    <hyperlink ref="B55" r:id="rId50" xr:uid="{F7DF44DB-1B41-404F-81A3-7AC81EE05A63}"/>
-    <hyperlink ref="B56" r:id="rId51" xr:uid="{D80DEE91-C66F-482C-9167-2EF8FCFC9C7C}"/>
-    <hyperlink ref="B61" r:id="rId52" xr:uid="{B89EDDE9-43F0-413A-BCC4-1985033AFFE9}"/>
-    <hyperlink ref="B63" r:id="rId53" xr:uid="{E3689BA1-5325-4CB6-AF82-C75005DF9AD8}"/>
-    <hyperlink ref="B60" r:id="rId54" xr:uid="{27C32D97-723A-49EC-9E07-AE6D55BCA76E}"/>
-    <hyperlink ref="B62" r:id="rId55" xr:uid="{66CFCC4F-B9FD-450D-B299-0977679F9F44}"/>
-    <hyperlink ref="B65" r:id="rId56" xr:uid="{2C12577D-5FBF-4996-B953-D85A399E34E2}"/>
-    <hyperlink ref="B64" r:id="rId57" xr:uid="{250B113A-BBF0-4765-BD52-F9C65955C15C}"/>
-    <hyperlink ref="B58" r:id="rId58" xr:uid="{ED359642-F18C-45EB-AEB0-79E5987941CB}"/>
-    <hyperlink ref="B57" r:id="rId59" xr:uid="{DF7C6DBA-903E-4F2E-9F05-8AACB763C49C}"/>
-    <hyperlink ref="B59" r:id="rId60" xr:uid="{0DE31A85-FC58-4475-AC30-556A4FDA1180}"/>
-    <hyperlink ref="B66" r:id="rId61" xr:uid="{A97C25F3-FACA-4DDB-8C40-453E6AF4ADB5}"/>
+    <hyperlink ref="B24" r:id="rId18" xr:uid="{926C4943-E630-4939-84A2-BEFC74A5F225}"/>
+    <hyperlink ref="B34" r:id="rId19" xr:uid="{7A5C2798-8BE5-4E96-BDEF-28F7CD2E738F}"/>
+    <hyperlink ref="B29" r:id="rId20" xr:uid="{4C7EFCDB-0E77-4C97-ACE6-C0CE8C394D37}"/>
+    <hyperlink ref="B32" r:id="rId21" xr:uid="{26F4AAB3-FFF1-4E0E-BF78-C8093E37AFBD}"/>
+    <hyperlink ref="B27" r:id="rId22" xr:uid="{13911792-9821-4E95-97DC-85E9B887C511}"/>
+    <hyperlink ref="B28" r:id="rId23" xr:uid="{69E5226C-7630-4695-9C81-A26D1377DE88}"/>
+    <hyperlink ref="B31" r:id="rId24" xr:uid="{CECD053F-7FD3-4B64-A49A-5D9C5A5F3BF9}"/>
+    <hyperlink ref="B30" r:id="rId25" xr:uid="{07B1DA00-5CF5-4122-9A5B-999FDE6C29EB}"/>
+    <hyperlink ref="B25" r:id="rId26" xr:uid="{5D22632C-FEEF-46B7-9865-41DA5B5CFDB3}"/>
+    <hyperlink ref="B33" r:id="rId27" xr:uid="{94D658C0-A0FE-4BF5-A204-C13F43B26FA9}"/>
+    <hyperlink ref="B26" r:id="rId28" xr:uid="{7C76A1DF-0C89-476C-8887-065E272C5483}"/>
+    <hyperlink ref="B36" r:id="rId29" xr:uid="{91F877AB-DA05-47DE-AA82-82BDE2FECF1D}"/>
+    <hyperlink ref="B45" r:id="rId30" xr:uid="{E80CAB3F-FB06-4D2A-BDC5-C95FF9ED0484}"/>
+    <hyperlink ref="B42" r:id="rId31" xr:uid="{F26B1534-C4A9-4963-967B-4D5E96E36851}"/>
+    <hyperlink ref="B46" r:id="rId32" xr:uid="{A82F6207-BA99-4836-8841-34BAE60666F0}"/>
+    <hyperlink ref="B38" r:id="rId33" xr:uid="{D84DD9F0-2D54-4A2C-879F-8C72F1F45A6E}"/>
+    <hyperlink ref="B39" r:id="rId34" xr:uid="{74083F87-F085-4AB8-8EA4-CD2E4611AD88}"/>
+    <hyperlink ref="B37" r:id="rId35" xr:uid="{5669B6F1-A30D-4310-8B87-82A6CDCC48B6}"/>
+    <hyperlink ref="B40" r:id="rId36" xr:uid="{96086732-E496-4DBB-8FA1-E150E110C6B7}"/>
+    <hyperlink ref="B43" r:id="rId37" xr:uid="{81AA84CD-D665-447C-823E-48B3E248604A}"/>
+    <hyperlink ref="B41" r:id="rId38" xr:uid="{C8935CA7-3220-467F-B000-6149E5E058D8}"/>
+    <hyperlink ref="B44" r:id="rId39" xr:uid="{474CDAE7-FC2C-4D4A-B7A1-C15D3453707C}"/>
+    <hyperlink ref="B48" r:id="rId40" xr:uid="{9576E6D8-C736-4763-91C8-7E183557C4C5}"/>
+    <hyperlink ref="B49" r:id="rId41" xr:uid="{A195B2E4-268B-4E5A-8FB4-56B97F8E4B99}"/>
+    <hyperlink ref="B50" r:id="rId42" xr:uid="{4BC7E6B9-1EE9-4FD4-BC5F-59BA867871B3}"/>
+    <hyperlink ref="B51" r:id="rId43" xr:uid="{589630DE-5DAD-45EC-8F36-D47477C02C73}"/>
+    <hyperlink ref="B52" r:id="rId44" xr:uid="{1DEFFFFE-C0A9-4491-A8DF-1834C0DEC3C1}"/>
+    <hyperlink ref="B53" r:id="rId45" xr:uid="{3EFBB842-4AFA-4A49-A1DF-C64565E21D5E}"/>
+    <hyperlink ref="B54" r:id="rId46" xr:uid="{AE4CC454-C550-4A47-96DE-5B64F3548C49}"/>
+    <hyperlink ref="B55" r:id="rId47" xr:uid="{DB8B1B41-3C6E-4F7F-9919-E2A0B1161647}"/>
+    <hyperlink ref="B56" r:id="rId48" xr:uid="{E6BEDB91-7182-4204-A234-9C695262B83B}"/>
+    <hyperlink ref="B57" r:id="rId49" xr:uid="{9F11431B-223D-4F6D-B269-253E92D3D8E2}"/>
+    <hyperlink ref="B58" r:id="rId50" xr:uid="{F7DF44DB-1B41-404F-81A3-7AC81EE05A63}"/>
+    <hyperlink ref="B59" r:id="rId51" xr:uid="{D80DEE91-C66F-482C-9167-2EF8FCFC9C7C}"/>
+    <hyperlink ref="B64" r:id="rId52" xr:uid="{B89EDDE9-43F0-413A-BCC4-1985033AFFE9}"/>
+    <hyperlink ref="B66" r:id="rId53" xr:uid="{E3689BA1-5325-4CB6-AF82-C75005DF9AD8}"/>
+    <hyperlink ref="B63" r:id="rId54" xr:uid="{27C32D97-723A-49EC-9E07-AE6D55BCA76E}"/>
+    <hyperlink ref="B65" r:id="rId55" xr:uid="{66CFCC4F-B9FD-450D-B299-0977679F9F44}"/>
+    <hyperlink ref="B68" r:id="rId56" xr:uid="{2C12577D-5FBF-4996-B953-D85A399E34E2}"/>
+    <hyperlink ref="B67" r:id="rId57" xr:uid="{250B113A-BBF0-4765-BD52-F9C65955C15C}"/>
+    <hyperlink ref="B61" r:id="rId58" xr:uid="{ED359642-F18C-45EB-AEB0-79E5987941CB}"/>
+    <hyperlink ref="B60" r:id="rId59" xr:uid="{DF7C6DBA-903E-4F2E-9F05-8AACB763C49C}"/>
+    <hyperlink ref="B62" r:id="rId60" xr:uid="{0DE31A85-FC58-4475-AC30-556A4FDA1180}"/>
+    <hyperlink ref="B23" r:id="rId61" xr:uid="{A1FAC0C9-F87F-4095-AB0F-7DA09DCED449}"/>
+    <hyperlink ref="B35" r:id="rId62" xr:uid="{110808D9-04E6-414C-82E6-5570FD935054}"/>
+    <hyperlink ref="B47" r:id="rId63" xr:uid="{86B04D21-DBD4-4B4C-9870-4CCB41BE6157}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Staff Juridico formulario, permisos, rutas JABG
</commit_message>
<xml_diff>
--- a/database/seeders/Usuarios.xlsx
+++ b/database/seeders/Usuarios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harold\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\servidor\Seguimiento\database\seeders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A9A10F-3F8E-419E-94D5-14C61C7A6378}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11DA5458-EA69-4AED-A37E-A591862A020E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{927018C0-BB9F-433A-9F90-4096039434DC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="157">
   <si>
     <t>nombre</t>
   </si>
@@ -475,13 +475,34 @@
   </si>
   <si>
     <t>maricela.love.07@gmail.com</t>
+  </si>
+  <si>
+    <t>Jorge Angel Becerril Gonzalez</t>
+  </si>
+  <si>
+    <t>desarrollador.f@osfem.gob.mx</t>
+  </si>
+  <si>
+    <t>Staff Juridico</t>
+  </si>
+  <si>
+    <t>STAFF</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>Consultor Administrativo</t>
+  </si>
+  <si>
+    <t>consultoradmin@osfem.gob.mx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -528,8 +549,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -584,8 +612,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -608,12 +641,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -711,9 +756,24 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1034,10 +1094,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{850591BD-AB77-48DF-A9A3-0C3060FEC0A7}">
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="I48" sqref="I48"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2384,7 +2444,7 @@
       <c r="A59" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B59" s="15" t="s">
+      <c r="B59" s="42" t="s">
         <v>123</v>
       </c>
       <c r="C59" s="24" t="s">
@@ -2608,6 +2668,52 @@
       </c>
       <c r="G68" s="29">
         <v>1632</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="37" t="s">
+        <v>150</v>
+      </c>
+      <c r="B69" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="C69" s="39" t="s">
+        <v>152</v>
+      </c>
+      <c r="D69" s="41">
+        <v>122100</v>
+      </c>
+      <c r="E69" s="40" t="s">
+        <v>152</v>
+      </c>
+      <c r="F69" s="40" t="s">
+        <v>153</v>
+      </c>
+      <c r="G69" s="40">
+        <v>1633</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="37" t="s">
+        <v>155</v>
+      </c>
+      <c r="B70" s="38" t="s">
+        <v>156</v>
+      </c>
+      <c r="C70" s="39" t="s">
+        <v>155</v>
+      </c>
+      <c r="D70" s="41">
+        <v>122000</v>
+      </c>
+      <c r="E70" s="40" t="s">
+        <v>155</v>
+      </c>
+      <c r="F70" s="40" t="s">
+        <v>154</v>
+      </c>
+      <c r="G70" s="40">
+        <v>1634</v>
       </c>
     </row>
   </sheetData>
@@ -2675,7 +2781,9 @@
     <hyperlink ref="B23" r:id="rId61" xr:uid="{A1FAC0C9-F87F-4095-AB0F-7DA09DCED449}"/>
     <hyperlink ref="B35" r:id="rId62" xr:uid="{110808D9-04E6-414C-82E6-5570FD935054}"/>
     <hyperlink ref="B47" r:id="rId63" xr:uid="{86B04D21-DBD4-4B4C-9870-4CCB41BE6157}"/>
+    <hyperlink ref="B69" r:id="rId64" xr:uid="{14150122-3177-4ABC-ACD9-B0B0497B02C1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId65"/>
 </worksheet>
 </file>
</xml_diff>